<commit_message>
ch09 - ch 11 airflow
</commit_message>
<xml_diff>
--- a/ApacheAirflow/Data Pipelines with Apache Airflow — копия.xlsx
+++ b/ApacheAirflow/Data Pipelines with Apache Airflow — копия.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3._Михайлов\Develop\PythonTraining\PythonTraining\ApacheAirflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3217C082-56FB-48B0-B838-B9B310EBE7DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2FED97-5CAA-488A-A680-63B2A6384453}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="15990" windowHeight="24720" xr2:uid="{322C65E7-B1BD-4309-A376-1D5B7C88940C}"/>
   </bookViews>
@@ -566,7 +566,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,14 +639,14 @@
         <v>35</v>
       </c>
       <c r="I2" s="1">
-        <f t="shared" ref="I2:I7" si="0">H2-G2</f>
+        <f t="shared" ref="I2:I8" si="0">H2-G2</f>
         <v>6</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
       <c r="K2" s="2">
-        <f t="shared" ref="K2:K7" si="1">I2/J2</f>
+        <f t="shared" ref="K2:K8" si="1">I2/J2</f>
         <v>6</v>
       </c>
       <c r="L2" t="s">
@@ -654,7 +654,7 @@
       </c>
       <c r="M2" s="2">
         <f>MEDIAN(I2:I18)</f>
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -697,7 +697,7 @@
       </c>
       <c r="M3" s="3">
         <f>MEDIAN(J2:J18)</f>
-        <v>6.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -740,7 +740,7 @@
       </c>
       <c r="M4" s="2">
         <f>MEDIAN(K2:K18)</f>
-        <v>5.2222222222222214</v>
+        <v>5.333333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -819,7 +819,7 @@
       </c>
       <c r="M6" s="2">
         <f>AVERAGE(I2:I18)</f>
-        <v>31</v>
+        <v>37.857142857142854</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -862,7 +862,7 @@
       </c>
       <c r="M7" s="2">
         <f>AVERAGE(J2:J18)</f>
-        <v>6.166666666666667</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -883,16 +883,29 @@
       <c r="F8" s="1">
         <v>7</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="K8" s="2"/>
+      <c r="G8" s="1">
+        <v>221</v>
+      </c>
+      <c r="H8" s="1">
+        <v>300</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="J8">
+        <v>12</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="1"/>
+        <v>6.583333333333333</v>
+      </c>
       <c r="L8" t="s">
         <v>31</v>
       </c>
       <c r="M8" s="2">
         <f>AVERAGE(K2:K18)</f>
-        <v>5.1924001924001919</v>
+        <v>5.3911049268192119</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -991,7 +1004,7 @@
       </c>
       <c r="M12">
         <f>SUM(J2:J18)</f>
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1021,7 +1034,7 @@
       </c>
       <c r="M13" s="2">
         <f>(MAX(B2:B20)-MAX(H2:H19))/M6</f>
-        <v>7.806451612903226</v>
+        <v>4.2792452830188683</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ch12 - ch15 airflow
</commit_message>
<xml_diff>
--- a/ApacheAirflow/Data Pipelines with Apache Airflow — копия.xlsx
+++ b/ApacheAirflow/Data Pipelines with Apache Airflow — копия.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3._Михайлов\Develop\PythonTraining\PythonTraining\ApacheAirflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2FED97-5CAA-488A-A680-63B2A6384453}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C713A3-F505-46DE-8545-2A89BACA33F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="15990" windowHeight="24720" xr2:uid="{322C65E7-B1BD-4309-A376-1D5B7C88940C}"/>
   </bookViews>
@@ -566,7 +566,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,22 +639,22 @@
         <v>35</v>
       </c>
       <c r="I2" s="1">
-        <f t="shared" ref="I2:I8" si="0">H2-G2</f>
-        <v>6</v>
+        <f>H2-G2+1</f>
+        <v>7</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
       <c r="K2" s="2">
-        <f t="shared" ref="K2:K8" si="1">I2/J2</f>
-        <v>6</v>
+        <f t="shared" ref="K2:K10" si="0">I2/J2</f>
+        <v>7</v>
       </c>
       <c r="L2" t="s">
         <v>22</v>
       </c>
       <c r="M2" s="2">
         <f>MEDIAN(I2:I18)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -665,7 +665,7 @@
         <v>46</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C14" si="2">B4-B3</f>
+        <f t="shared" ref="C3:C14" si="1">B4-B3</f>
         <v>20</v>
       </c>
       <c r="D3" s="1">
@@ -682,15 +682,15 @@
         <v>52</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <f t="shared" ref="I3:I10" si="2">H3-G3+1</f>
+        <v>17</v>
       </c>
       <c r="J3">
         <v>3</v>
       </c>
       <c r="K3" s="2">
-        <f t="shared" si="1"/>
-        <v>5.333333333333333</v>
+        <f t="shared" si="0"/>
+        <v>5.666666666666667</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -708,7 +708,7 @@
         <v>66</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="D4" s="1">
@@ -725,22 +725,22 @@
         <v>85</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" si="0"/>
-        <v>32</v>
+        <f t="shared" si="2"/>
+        <v>33</v>
       </c>
       <c r="J4">
         <v>6</v>
       </c>
       <c r="K4" s="2">
-        <f t="shared" si="1"/>
-        <v>5.333333333333333</v>
+        <f t="shared" si="0"/>
+        <v>5.5</v>
       </c>
       <c r="L4" t="s">
         <v>20</v>
       </c>
       <c r="M4" s="2">
         <f>MEDIAN(K2:K18)</f>
-        <v>5.333333333333333</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -751,7 +751,7 @@
         <v>86</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="D5" s="1">
@@ -768,15 +768,15 @@
         <v>132</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" si="0"/>
-        <v>46</v>
+        <f t="shared" si="2"/>
+        <v>47</v>
       </c>
       <c r="J5">
         <v>9</v>
       </c>
       <c r="K5" s="2">
-        <f t="shared" si="1"/>
-        <v>5.1111111111111107</v>
+        <f t="shared" si="0"/>
+        <v>5.2222222222222223</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -787,7 +787,7 @@
         <v>111</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="D6" s="1">
@@ -804,22 +804,22 @@
         <v>163</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="0"/>
-        <v>30</v>
+        <f t="shared" si="2"/>
+        <v>31</v>
       </c>
       <c r="J6">
         <v>7</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" si="1"/>
-        <v>4.2857142857142856</v>
+        <f t="shared" si="0"/>
+        <v>4.4285714285714288</v>
       </c>
       <c r="L6" t="s">
         <v>29</v>
       </c>
       <c r="M6" s="2">
         <f>AVERAGE(I2:I18)</f>
-        <v>37.857142857142854</v>
+        <v>40.555555555555557</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -830,7 +830,7 @@
         <v>141</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="D7" s="1">
@@ -847,15 +847,15 @@
         <v>220</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="0"/>
-        <v>56</v>
+        <f t="shared" si="2"/>
+        <v>57</v>
       </c>
       <c r="J7">
         <v>11</v>
       </c>
       <c r="K7" s="2">
-        <f t="shared" si="1"/>
-        <v>5.0909090909090908</v>
+        <f t="shared" si="0"/>
+        <v>5.1818181818181817</v>
       </c>
       <c r="L7" t="s">
         <v>30</v>
@@ -873,7 +873,7 @@
         <v>161</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="D8" s="1">
@@ -890,22 +890,22 @@
         <v>300</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="0"/>
-        <v>79</v>
+        <f t="shared" si="2"/>
+        <v>80</v>
       </c>
       <c r="J8">
         <v>12</v>
       </c>
       <c r="K8" s="2">
-        <f t="shared" si="1"/>
-        <v>6.583333333333333</v>
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
       </c>
       <c r="L8" t="s">
         <v>31</v>
       </c>
       <c r="M8" s="2">
         <f>AVERAGE(K2:K18)</f>
-        <v>5.3911049268192119</v>
+        <v>5.6699535032868358</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -916,7 +916,7 @@
         <v>183</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="D9" s="1">
@@ -926,10 +926,23 @@
       <c r="F9" s="1">
         <v>8</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="K9" s="2"/>
+      <c r="G9" s="1">
+        <v>301</v>
+      </c>
+      <c r="H9" s="1">
+        <v>312</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -939,7 +952,7 @@
         <v>212</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="D10" s="1">
@@ -949,10 +962,23 @@
       <c r="F10" s="1">
         <v>9</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="K10" s="2"/>
+      <c r="G10" s="1">
+        <v>313</v>
+      </c>
+      <c r="H10" s="1">
+        <v>393</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="2"/>
+        <v>81</v>
+      </c>
+      <c r="J10">
+        <v>11</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="0"/>
+        <v>7.3636363636363633</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -962,7 +988,7 @@
         <v>246</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="D11" s="1">
@@ -985,7 +1011,7 @@
         <v>281</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="D12" s="1">
@@ -1004,7 +1030,7 @@
       </c>
       <c r="M12">
         <f>SUM(J2:J18)</f>
-        <v>49</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1015,7 +1041,7 @@
         <v>307</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="D13" s="1">
@@ -1034,7 +1060,7 @@
       </c>
       <c r="M13" s="2">
         <f>(MAX(B2:B20)-MAX(H2:H19))/M6</f>
-        <v>4.2792452830188683</v>
+        <v>1.7013698630136986</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1045,7 +1071,7 @@
         <v>348</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="D14" s="1">

</xml_diff>